<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  7785
Describing values allowed for enumerations
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -4098,7 +4098,7 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -4926,7 +4926,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -5202,7 +5202,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -5478,7 +5478,7 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>genomeSequencing</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  7894
Updating Cultivability default value to an authorized value
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -1482,6 +1482,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"GET,POST"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"GET,POST"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1661,6 +1669,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ENA,GenBank"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2048,6 +2061,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Virus,Bacterium,Fungus,Protozoan,Viroid,Prion"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Animal,Human,Plant"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3283,6 +3304,26 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Soluble,Inclusion bodies"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Denatured,Refolded"</formula1>
+    </dataValidation>
+    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"E. coli,Insect cells,Mammalian cells"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Functionally characterized,No functional characterization"</formula1>
+    </dataValidation>
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Greater than 95 percent,Unpurified expression host lysate or partly purified protein"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Enzymatic,Antigenic"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3585,6 +3626,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not sequenced,Partly sequenced,Fully sequenced"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4273,6 +4319,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="T2:T1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4549,6 +4609,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -4825,6 +4899,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5101,6 +5189,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5377,6 +5479,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5653,6 +5769,20 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Cultivable,Uncultivable,Inactivated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Infectivity tested,Infectivity tested and quantified,Non cultivable sample, infectivity cannot be tested"</formula1>
+    </dataValidation>
+    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Not applicable,Not required,Required for customers in the EU,Required"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Complete genome,Complete coding sequence,Partial sequence"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  8498
Reducing variation of a same slot between classes, adding complementary sheets for slots details, domains and classes
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -3832,2423 +3832,2525 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>complementaryDocument</t>
         </is>
       </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>coInfectingViruses</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>contaminationWithCoInfectingViruses</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>mycoplasmicContent</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>hasIATAClassification</t>
         </is>
       </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>shippingConditions</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>materialSafetyDataSheet</t>
         </is>
       </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>originator</t>
         </is>
       </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>storageConditions</t>
         </is>
       </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AY1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>suspectedEpidemiologicalOrigin</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>isolationHost</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>productionCellLine</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>propagationHost</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>transmissionMethod</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>cultivability</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>clinicalInformation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>infectivity</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>infectivityTest</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>isolationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>isolationConditions</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>letterOfAuthority</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>hasIATAClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
           <t>thirdPartyDistributionConsent</t>
         </is>
       </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>accessPointURL</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>refSKU</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>relatedDOI</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canItBeUsedToProduceGMO</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>msdsContact</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>physicalChemicalProperties</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hazardsIdentification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>firstAidMeasures</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fireFightingMeasures</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>accidentalReleaseMeasures</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>handlingAndStorage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exposureControlsPersonalProtection</t>
+        </is>
+      </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>usageRestrictions</t>
+          <t>stabilityAndReactivity</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>toxicologicalInformation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>ecologicalInformation</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>disposalConsiderations</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>transportInformation</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>regulatoryInformation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>furtherInformation</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>termDataProvider</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>term</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BB1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>coInfectingViruses</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>contaminationWithCoInfectingViruses</t>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mycoplasmicContent</t>
+          <t>contentURL</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>biologicalMaterialOrigin</t>
+          <t>format</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>suspectedEpidemiologicalOrigin</t>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentURL</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentURL</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentURL</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>altText</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>contentURL</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>format</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>isolationHost</t>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>telephone</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>streetAddress</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>addressLocality</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>productionCellLine</t>
+          <t>addressRegion</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>propagationHost</t>
+          <t>postalCode</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>transmissionMethod</t>
+          <t>addressCountry</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
+          <t>oRCIDiD</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
-        </is>
-      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>isolationHost</t>
+          <t>resourceURL</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>productionCellLine</t>
+          <t>licensingOrAttribution</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>propagationHost</t>
+          <t>logo</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>certificationDocument</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>resourceURL</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>weight</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
+          <t>inVocabulary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inVocabulary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>isolationHost</t>
+          <t>name</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>productionCellLine</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>propagationHost</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>isolationHost</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>productionCellLine</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>propagationHost</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>isolationHost</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>productionCellLine</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>propagationHost</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AY1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>isolationHost</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>productionCellLine</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>propagationHost</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>hasIATAClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>accessPointURL</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>refSKU</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>relatedDOI</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canItBeUsedToProduceGMO</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>msdsContact</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>physicalChemicalProperties</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>hazardsIdentification</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>firstAidMeasures</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>fireFightingMeasures</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>accidentalReleaseMeasures</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>handlingAndStorage</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>exposureControlsPersonalProtection</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>stabilityAndReactivity</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>toxicologicalInformation</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>ecologicalInformation</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>disposalConsiderations</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>transportInformation</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>regulatoryInformation</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>furtherInformation</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>termDataProvider</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>term</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contentURL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contentURL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contentURL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contentURL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>altText</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>contentURL</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>telephone</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>streetAddress</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>addressLocality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>addressRegion</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>postalCode</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>addressCountry</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>oRCIDiD</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>resourceURL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>licensingOrAttribution</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>certificationDocument</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>resourceURL</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>inVocabulary</t>
         </is>
       </c>
@@ -6256,106 +6358,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inVocabulary</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inVocabulary</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  8702
Stripping spaces in prefixes and class identifiers
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -56,8 +56,8 @@
     <sheet name="Antibody" sheetId="47" state="visible" r:id="rId47"/>
     <sheet name="Hybridoma" sheetId="48" state="visible" r:id="rId48"/>
     <sheet name="Protein" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="Nucleic Acid" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet name="Detection Kit" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="NucleicAcid" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="DetectionKit" sheetId="51" state="visible" r:id="rId51"/>
     <sheet name="Bundle" sheetId="52" state="visible" r:id="rId52"/>
     <sheet name="Virus" sheetId="53" state="visible" r:id="rId53"/>
     <sheet name="Bacterium" sheetId="54" state="visible" r:id="rId54"/>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  8979
Replacing Protein Tag by Sequence Tag for better semantic representation according to Pr B.Coutard
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -21,7 +21,7 @@
     <sheet name="Journal" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="PdbReference" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="Keyword" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="ProteinTag" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="TagSequence" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="SpecialFeature" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="ExpressionVector" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="PlasmidSelection" sheetId="18" state="visible" r:id="rId18"/>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>proteinTag</t>
+          <t>tagSequence</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>proteinTag</t>
+          <t>tagSequence</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  9489
Reporting MSDS Class name upgrade in related properties
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -66,15 +66,14 @@
     <sheet name="Viroid" sheetId="57" state="visible" r:id="rId57"/>
     <sheet name="Prion" sheetId="58" state="visible" r:id="rId58"/>
     <sheet name="MaterialSafetyDataSheet" sheetId="59" state="visible" r:id="rId59"/>
-    <sheet name="MSDS" sheetId="60" state="visible" r:id="rId60"/>
-    <sheet name="Data" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet name="Document" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet name="Audio" sheetId="63" state="visible" r:id="rId63"/>
-    <sheet name="Video" sheetId="64" state="visible" r:id="rId64"/>
-    <sheet name="Image" sheetId="65" state="visible" r:id="rId65"/>
-    <sheet name="ContactPoint" sheetId="66" state="visible" r:id="rId66"/>
-    <sheet name="License" sheetId="67" state="visible" r:id="rId67"/>
-    <sheet name="Certification" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet name="Data" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet name="Document" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet name="Audio" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet name="Video" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet name="Image" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet name="ContactPoint" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet name="License" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet name="Certification" sheetId="67" state="visible" r:id="rId67"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5764,14 +5763,92 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>materialSafetyContact</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>physicalChemicalProperties</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>hazardsIdentification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>firstAidMeasures</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fireFightingMeasures</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>accidentalReleaseMeasures</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>handlingAndStorage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exposureControlsPersonalProtection</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stabilityAndReactivity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>toxicologicalInformation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>ecologicalInformation</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>disposalConsiderations</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>transportInformation</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>regulatoryInformation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>furtherInformation</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5828,97 +5905,307 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>materialSafetyContact</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>physicalChemicalProperties</t>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>hazardsIdentification</t>
+          <t>contentUrl</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>firstAidMeasures</t>
+          <t>format</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>fireFightingMeasures</t>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentUrl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentUrl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentUrl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>altText</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>contentUrl</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>format</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>accidentalReleaseMeasures</t>
+          <t>license</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>telephone</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>streetAddress</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>addressLocality</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>handlingAndStorage</t>
+          <t>addressRegion</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>exposureControlsPersonalProtection</t>
+          <t>postalCode</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>stabilityAndReactivity</t>
+          <t>addressCountry</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>toxicologicalInformation</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>ecologicalInformation</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>disposalConsiderations</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>transportInformation</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>regulatoryInformation</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>furtherInformation</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>orcidId</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5935,7 +6222,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>title</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5945,26 +6232,26 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>contentUrl</t>
+          <t>resourceUrl</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>licensingOrAttribution</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>logo</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5981,7 +6268,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>title</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5991,373 +6278,169 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>contentUrl</t>
+          <t>logo</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>certificationDocument</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>resourceUrl</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inVocabulary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>contentUrl</t>
+          <t>title</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inVocabulary</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sourceOfInformation</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>contentUrl</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>altText</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>contentUrl</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>format</t>
+          <t>weight</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>license</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>telephone</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>streetAddress</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>addressLocality</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>addressRegion</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>postalCode</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>addressCountry</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>orcidId</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>resourceUrl</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>licensingOrAttribution</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>certificationDocument</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>resourceUrl</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>inVocabulary</t>
         </is>
       </c>
@@ -6365,106 +6448,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inVocabulary</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sourceOfInformation</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>weight</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>inVocabulary</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  9841
Improve unit cost handling
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -2488,7 +2488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2539,110 +2539,120 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -2659,7 +2669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2735,110 +2745,120 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -2855,7 +2875,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2956,110 +2976,120 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -3076,7 +3106,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3182,110 +3212,120 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -3302,7 +3342,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3448,110 +3488,120 @@
       </c>
       <c r="AB1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -3619,7 +3669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:AY1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3765,110 +3815,120 @@
       </c>
       <c r="AB1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -3885,7 +3945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3981,110 +4041,120 @@
       </c>
       <c r="R1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -4101,7 +4171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4182,110 +4252,120 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -4302,7 +4382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4483,110 +4563,120 @@
       </c>
       <c r="AI1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -4603,7 +4693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4769,110 +4859,120 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -4889,7 +4989,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5055,110 +5155,120 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -5175,7 +5285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5341,110 +5451,120 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -5461,7 +5581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5627,110 +5747,120 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
@@ -5747,7 +5877,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5913,110 +6043,120 @@
       </c>
       <c r="AF1" t="inlineStr">
         <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  9907
Introduce ClinicalGroup class
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -37,43 +37,44 @@
     <sheet name="Variant" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="TaxonomicRank" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="Taxon" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="ExternalRelatedReference" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="Sequence" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="SequenceReference" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PersonOrOrganization" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="Person" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="Organization" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="ReasearchInfrastructure" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="Provider" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="Originator" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="BiologicalMaterialOrigin" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="NaturalPartOrigin" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="SyntheticPartOrigin" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="RecombinantPartIdentification" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="Collection" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="Service" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="Product" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="Antibody" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="Hybridoma" sheetId="48" state="visible" r:id="rId48"/>
-    <sheet name="Protein" sheetId="49" state="visible" r:id="rId49"/>
-    <sheet name="NucleicAcid" sheetId="50" state="visible" r:id="rId50"/>
-    <sheet name="DetectionKit" sheetId="51" state="visible" r:id="rId51"/>
-    <sheet name="Bundle" sheetId="52" state="visible" r:id="rId52"/>
-    <sheet name="Virus" sheetId="53" state="visible" r:id="rId53"/>
-    <sheet name="Bacterium" sheetId="54" state="visible" r:id="rId54"/>
-    <sheet name="Fungus" sheetId="55" state="visible" r:id="rId55"/>
-    <sheet name="Protozoan" sheetId="56" state="visible" r:id="rId56"/>
-    <sheet name="Viroid" sheetId="57" state="visible" r:id="rId57"/>
-    <sheet name="Prion" sheetId="58" state="visible" r:id="rId58"/>
-    <sheet name="MaterialSafetyDataSheet" sheetId="59" state="visible" r:id="rId59"/>
-    <sheet name="Data" sheetId="60" state="visible" r:id="rId60"/>
-    <sheet name="Document" sheetId="61" state="visible" r:id="rId61"/>
-    <sheet name="Audio" sheetId="62" state="visible" r:id="rId62"/>
-    <sheet name="Video" sheetId="63" state="visible" r:id="rId63"/>
-    <sheet name="Image" sheetId="64" state="visible" r:id="rId64"/>
-    <sheet name="ContactPoint" sheetId="65" state="visible" r:id="rId65"/>
-    <sheet name="License" sheetId="66" state="visible" r:id="rId66"/>
-    <sheet name="Certification" sheetId="67" state="visible" r:id="rId67"/>
+    <sheet name="ClinicalGroup" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="ExternalRelatedReference" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Sequence" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="SequenceReference" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PersonOrOrganization" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="Person" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="Organization" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="ReasearchInfrastructure" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="Provider" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="Originator" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="BiologicalMaterialOrigin" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="NaturalPartOrigin" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SyntheticPartOrigin" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="RecombinantPartIdentification" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="Collection" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="Service" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Product" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="Antibody" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="Hybridoma" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="Protein" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="NucleicAcid" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet name="DetectionKit" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet name="Bundle" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet name="Virus" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet name="Bacterium" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="Fungus" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet name="Protozoan" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet name="Viroid" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet name="Prion" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet name="MaterialSafetyDataSheet" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet name="Data" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet name="Document" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet name="Audio" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet name="Video" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet name="Image" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet name="ContactPoint" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet name="License" sheetId="67" state="visible" r:id="rId67"/>
+    <sheet name="Certification" sheetId="68" state="visible" r:id="rId68"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1938,7 +1939,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1949,35 +1950,45 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>alternateName</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>referenceLabel</t>
+          <t>taxon</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>referenceProviderPrefix</t>
+          <t>title</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>referenceProviderName</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>weight</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>inVocabulary</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -1994,7 +2005,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,25 +2016,35 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>sequenceReference</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>sequenceFasta</t>
+          <t>referenceLabel</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>referenceProviderPrefix</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>referenceProviderName</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -2051,12 +2072,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>accessionNumber</t>
+          <t>sequenceReference</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>sequenceProvider</t>
+          <t>sequenceFasta</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -2081,6 +2102,52 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>accessionNumber</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequenceProvider</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2141,7 +2208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2197,82 +2264,6 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>alternateName</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>country</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>rorId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>homePage</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -2365,7 +2356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2376,60 +2367,55 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>memberOfRi</t>
+          <t>alternateName</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alternateName</t>
+          <t>country</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>country</t>
+          <t>rorId</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>rorId</t>
+          <t>name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>description</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>homePage</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>homePage</t>
+          <t>contactPoint</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>contactPoint</t>
+          <t>logo</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>logo</t>
+          <t>keyword</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>keyword</t>
+          <t>dateIssued</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -2446,7 +2432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2457,40 +2443,60 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>memberOfRi</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rorId</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>homePage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>logo</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -2593,6 +2599,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>homePage</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2638,7 +2705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2709,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2765,7 +2832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2811,7 +2878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2872,7 +2939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3063,7 +3130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3279,7 +3346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3520,7 +3587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3756,292 +3823,6 @@
         </is>
       </c>
       <c r="AS1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>relatedPdb</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>specialFeature</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>tagSequence</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>domain</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>expressedAs</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>inclusionBodiesType</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>expressionSystem</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>functionalCharacterization</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>functionalAndTechnicalDescription</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>proteinPurification</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>tagStatusOfTheSolubilizedProtein</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>typeOfFunctionalCharacterization</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>iataClassification</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>accessPointUrl</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>refSku</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>unitCostCurrency</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>unitCostNote</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>doi</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>canBeUsedToProduceGmo</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -4135,67 +3916,67 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>genBankFileOfTheConstruct</t>
+          <t>sequence</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>sequence</t>
+          <t>relatedPdb</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>clonedNucleicAcid</t>
+          <t>specialFeature</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>clonedIntoPlasmid</t>
+          <t>tagSequence</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>plasmidSelection</t>
+          <t>domain</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>tagSequence</t>
+          <t>expressedAs</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>regionEncompassedInThisProduct</t>
+          <t>inclusionBodiesType</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>mutationObserved</t>
+          <t>expressionSystem</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>observedMutations</t>
+          <t>functionalCharacterization</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>identificationTechnique</t>
+          <t>functionalAndTechnicalDescription</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>sequencing</t>
+          <t>proteinPurification</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>titer</t>
+          <t>tagStatusOfTheSolubilizedProtein</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>sequenceChecked</t>
+          <t>typeOfFunctionalCharacterization</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
@@ -4400,6 +4181,292 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:BA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biologicalMaterialOrigin</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>genBankFileOfTheConstruct</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>clonedNucleicAcid</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>clonedIntoPlasmid</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>plasmidSelection</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tagSequence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>regionEncompassedInThisProduct</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>mutationObserved</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>observedMutations</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>identificationTechnique</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>sequencing</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>sequenceChecked</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>iataClassification</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>accessPointUrl</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>refSku</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>canBeUsedToProduceGmo</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4635,7 +4702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4856,7 +4923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5167,312 +5234,6 @@
         </is>
       </c>
       <c r="BH1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:BE1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>biologicalMaterialOrigin</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>suspectedEpidemiologicalOrigin</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>isolationHost</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>productionCellLine</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>propagationHost</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>transmissionMethod</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>cultivability</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>clinicalInformation</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>identificationTechnique</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>infectivity</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>infectivityTest</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>isolationTechnique</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>isolationConditions</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>letterOfAuthority</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>passage</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>genomeSequencing</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>iataClassification</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>accessPointUrl</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>refSku</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>unitCostCurrency</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>unitCostNote</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>doi</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>canBeUsedToProduceGmo</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -6713,7 +6474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6724,90 +6485,285 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>materialSafetyContact</t>
+          <t>biologicalMaterialOrigin</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>physicalChemicalProperties</t>
+          <t>suspectedEpidemiologicalOrigin</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>hazardsIdentification</t>
+          <t>isolationHost</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>firstAidMeasures</t>
+          <t>productionCellLine</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>fireFightingMeasures</t>
+          <t>propagationHost</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>accidentalReleaseMeasures</t>
+          <t>transmissionMethod</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>handlingAndStorage</t>
+          <t>sequence</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>exposureControlsPersonalProtection</t>
+          <t>cultivability</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>stabilityAndReactivity</t>
+          <t>clinicalInformation</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>toxicologicalInformation</t>
+          <t>identificationTechnique</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ecologicalInformation</t>
+          <t>infectivity</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>disposalConsiderations</t>
+          <t>infectivityTest</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>transportInformation</t>
+          <t>isolationTechnique</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>regulatoryInformation</t>
+          <t>isolationConditions</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>furtherInformation</t>
+          <t>letterOfAuthority</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>passage</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>genomeSequencing</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>titer</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>iataClassification</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>accessPointUrl</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>refSku</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>canBeUsedToProduceGmo</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -6885,7 +6841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6896,40 +6852,90 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>materialSafetyContact</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>physicalChemicalProperties</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>contentUrl</t>
+          <t>hazardsIdentification</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>firstAidMeasures</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>license</t>
+          <t>fireFightingMeasures</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>accidentalReleaseMeasures</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>handlingAndStorage</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exposureControlsPersonalProtection</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>stabilityAndReactivity</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>toxicologicalInformation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>ecologicalInformation</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>disposalConsiderations</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>transportInformation</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>regulatoryInformation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>furtherInformation</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -7129,6 +7135,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contentUrl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>license</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7189,7 +7256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7265,67 +7332,6 @@
         </is>
       </c>
       <c r="M1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>resourceUrl</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>licensingOrAttribution</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>logo</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
@@ -7363,6 +7369,67 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>resourceUrl</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>licensingOrAttribution</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>logo</t>
         </is>
       </c>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  10013
Improve Taxon entity and deprecate previouslyKnownAs in favor of alternateName
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -2078,7 +2078,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2104,65 +2104,70 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>externalEquivalentTaxon</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>taxonomicId</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>taxonomicNodeId</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>previouslyKnownAs</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>externalEquivalentTaxon</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>taxonomicId</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>taxonomicNodeId</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>weight</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>inVocabulary</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  10123
Implement Funding Source
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -75,6 +75,7 @@
     <sheet name="ContactPoint" sheetId="66" state="visible" r:id="rId66"/>
     <sheet name="License" sheetId="67" state="visible" r:id="rId67"/>
     <sheet name="Certification" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet name="FundingSource" sheetId="69" state="visible" r:id="rId69"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3350,7 +3351,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ1"/>
+  <dimension ref="A1:AK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3501,40 +3502,45 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -3551,7 +3557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AP1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3727,40 +3733,45 @@
       </c>
       <c r="AH1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -3772,257 +3783,6 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AT1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>productionSystem</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>antibodyPurifiedByAffinity</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>specificityDocumented</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>targetedAntigen</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sequenceReference</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>iataClassification</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>accessPointUrl</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>refSku</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>unitCostCurrency</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>unitCostNote</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>doi</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>canBeUsedToProduceGmo</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>iri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4039,6 +3799,262 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>productionSystem</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>antibodyPurifiedByAffinity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>specificityDocumented</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>targetedAntigen</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sequenceReference</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>iataClassification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>accessPointUrl</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>refSku</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>canBeUsedToProduceGmo</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AV1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>hybridomaDescription</t>
         </is>
       </c>
@@ -4234,40 +4250,45 @@
       </c>
       <c r="AN1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4355,7 +4376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4601,40 +4622,45 @@
       </c>
       <c r="AV1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4651,7 +4677,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4897,40 +4923,45 @@
       </c>
       <c r="AV1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4947,7 +4978,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5143,40 +5174,45 @@
       </c>
       <c r="AL1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5193,7 +5229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5374,40 +5410,45 @@
       </c>
       <c r="AI1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5424,7 +5465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BK1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5705,40 +5746,45 @@
       </c>
       <c r="BC1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5755,7 +5801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6021,40 +6067,45 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6071,7 +6122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6337,40 +6388,45 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6387,7 +6443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6653,40 +6709,45 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6703,7 +6764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6969,40 +7030,45 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -7019,7 +7085,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7285,40 +7351,45 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -8119,6 +8190,92 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fundingProgram</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>grantNumber</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>funder</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fundingPeriodStart</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>fundingPeriodEnd</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>eligibilityCriteria</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  10142
Add preparationTechnique property to Product
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -3557,7 +3557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3603,175 +3603,180 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -3783,262 +3788,6 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AU1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>productionSystem</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>antibodyPurifiedByAffinity</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>specificityDocumented</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>targetedAntigen</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>sequenceReference</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>iataClassification</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>shippingConditions</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>materialSafetyDataSheet</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>originator</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>storageConditions</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>thirdPartyDistributionConsent</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>usageRestrictions</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>accessPointUrl</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>refSku</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>unitDefinition</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>additionalCategory</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>unitCost</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>unitCostCurrency</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>unitCostNote</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>qualityGrading</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>pathogenIdentification</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>doi</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>riskGroup</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>biosafetyRestrictions</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>canBeUsedToProduceGmo</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>provider</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>availability</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>complementaryDocument</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>technicalRecommendation</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>productPicture</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>externalRelatedReference</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>certification</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>internalReference</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>contactPoint</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>fundingSource</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>version</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>dateIssued</t>
-        </is>
-      </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>dateModified</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>identifier</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>iri</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4055,6 +3804,267 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>productionSystem</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>antibodyPurifiedByAffinity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>specificityDocumented</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>targetedAntigen</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sequenceReference</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>iataClassification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>shippingConditions</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>materialSafetyDataSheet</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>originator</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>storageConditions</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>thirdPartyDistributionConsent</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>usageRestrictions</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>accessPointUrl</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>refSku</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>unitDefinition</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>additionalCategory</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>unitCost</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>unitCostCurrency</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>unitCostNote</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>qualityGrading</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pathogenIdentification</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>doi</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>riskGroup</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>biosafetyRestrictions</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>canBeUsedToProduceGmo</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>provider</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>collection</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>keywords</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>availability</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>complementaryDocument</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>technicalRecommendation</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>productPicture</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>externalRelatedReference</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>certification</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>internalReference</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>note</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>contactPoint</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>fundingSource</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>dateIssued</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>dateModified</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>identifier</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>iri</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AW1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>hybridomaDescription</t>
         </is>
       </c>
@@ -4120,175 +4130,180 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4376,7 +4391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4492,175 +4507,180 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4677,7 +4697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4793,175 +4813,180 @@
       </c>
       <c r="V1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4978,7 +5003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5044,175 +5069,180 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5229,7 +5259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5280,175 +5310,180 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5465,7 +5500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK1"/>
+  <dimension ref="A1:BL1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5616,175 +5651,180 @@
       </c>
       <c r="AC1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -5801,7 +5841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5937,175 +5977,180 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6122,7 +6167,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6258,175 +6303,180 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6443,7 +6493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6579,175 +6629,180 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -6764,7 +6819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6900,175 +6955,180 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -7085,7 +7145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH1"/>
+  <dimension ref="A1:BI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7221,175 +7281,180 @@
       </c>
       <c r="Z1" t="inlineStr">
         <is>
+          <t>preparationTechnique</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -8196,7 +8261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8247,25 +8312,30 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  10720
Add antibodyType, antibodyCharacterizationMethod, and antibodyCharacterizationObservation properties to Antibody class
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -3870,7 +3870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:AZ1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3906,220 +3906,235 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>antibodyType</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>antibodyCharacterizationMethod</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>antibodyCharacterizationObservation</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>iataClassification</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>shippingConditions</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>materialSafetyDataSheet</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>originator</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>storageConditions</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>thirdPartyDistributionConsent</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>usageRestrictions</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>preparationTechnique</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>biosafetyLevel</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4207,7 +4222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4248,220 +4263,235 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>antibodyType</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>antibodyCharacterizationMethod</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>antibodyCharacterizationObservation</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>iataClassification</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>shippingConditions</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>materialSafetyDataSheet</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>originator</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>storageConditions</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>thirdPartyDistributionConsent</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>usageRestrictions</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>preparationTechnique</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>biosafetyLevel</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>

</xml_diff>

<commit_message>
CI Build: Synchronisation of the project's models with the google sheet metadata version  10742
Add antibodySpecificity property
</commit_message>
<xml_diff>
--- a/models/subsidiary_models/excel/evora_schema.xlsx
+++ b/models/subsidiary_models/excel/evora_schema.xlsx
@@ -3870,7 +3870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3896,245 +3896,250 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>antibodySpecificity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>targetedAntigen</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>sequenceReference</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>antibodyType</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>antibodyCharacterizationMethod</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>antibodyCharacterizationObservation</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>iataClassification</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>shippingConditions</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>materialSafetyDataSheet</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>originator</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>storageConditions</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>thirdPartyDistributionConsent</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>usageRestrictions</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>preparationTechnique</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>biosafetyLevel</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>
@@ -4222,7 +4227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BB1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4253,245 +4258,250 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>antibodySpecificity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>targetedAntigen</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>sequenceReference</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>antibodyType</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>antibodyCharacterizationMethod</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>antibodyCharacterizationObservation</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>iataClassification</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>shippingConditions</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>materialSafetyDataSheet</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>originator</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>storageConditions</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>thirdPartyDistributionConsent</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>usageRestrictions</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>preparationTechnique</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>accessPointUrl</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>refSku</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>unitDefinition</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>additionalCategory</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>unitCost</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>unitCostCurrency</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>unitCostNote</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>qualityGrading</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>pathogenIdentification</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>doi</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>riskGroup</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>biosafetyLevel</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>biosafetyRestrictions</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>canBeUsedToProduceGmo</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>provider</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>collection</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>keywords</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>availability</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>complementaryDocument</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>technicalRecommendation</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>productPicture</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>externalRelatedReference</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>certification</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>internalReference</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>contactPoint</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>fundingSource</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>version</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>keyword</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>dateIssued</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>dateModified</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>iri</t>
         </is>

</xml_diff>